<commit_message>
add countFrequency and more configuration
</commit_message>
<xml_diff>
--- a/IEEE_Member_App_20-21.xlsx
+++ b/IEEE_Member_App_20-21.xlsx
@@ -1,19 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasnguyen/Desktop/Github/TkWahldgets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DE3FD6-C9CB-9244-9CCF-02CFBEBB8D06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23860" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="GM1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="GM2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="GM3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="GM4" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Student Advisory Week" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Freshmen Roadmap" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Career Fair Bootcamp Volunteers" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Career Fair Bootcamp Attendees" sheetId="8" r:id="rId11"/>
+    <sheet name="GM1" sheetId="1" r:id="rId1"/>
+    <sheet name="GM2" sheetId="2" r:id="rId2"/>
+    <sheet name="GM3" sheetId="3" r:id="rId3"/>
+    <sheet name="GM4" sheetId="4" r:id="rId4"/>
+    <sheet name="Student Advisory Week" sheetId="5" r:id="rId5"/>
+    <sheet name="Freshmen Roadmap" sheetId="6" r:id="rId6"/>
+    <sheet name="Career Fair Bootcamp Volunteers" sheetId="7" r:id="rId7"/>
+    <sheet name="Career Fair Bootcamp Attendees" sheetId="8" r:id="rId8"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1640,23 +1660,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1664,7 +1687,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1698,86 +1721,57 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="20" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1967,26 +1961,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="15" width="21.57"/>
+    <col min="1" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2015,9 +2016,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>44072.80618347222</v>
+        <v>44072.806183472218</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -2026,7 +2027,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>1625156.0</v>
+        <v>1625156</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2044,7 +2045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>44076.533342002316</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>5156.0</v>
+        <v>5156</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -2073,9 +2074,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44076.74747372685</v>
+        <v>44076.747473726849</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
@@ -2084,7 +2085,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="2">
-        <v>4175.0</v>
+        <v>4175</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
@@ -2102,9 +2103,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44076.74766824074</v>
+        <v>44076.747668240743</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -2113,7 +2114,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="2">
-        <v>5641.0</v>
+        <v>5641</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>23</v>
@@ -2131,9 +2132,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44076.74792679398</v>
+        <v>44076.747926793978</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -2154,9 +2155,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
-        <v>44076.74807796296</v>
+        <v>44076.748077962962</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
@@ -2165,7 +2166,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2">
-        <v>5510.0</v>
+        <v>5510</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>32</v>
@@ -2180,7 +2181,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44076.748192175924</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="2">
-        <v>6921.0</v>
+        <v>6921</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>38</v>
@@ -2203,9 +2204,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44076.74873232639</v>
+        <v>44076.748732326392</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>39</v>
@@ -2229,9 +2230,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>44076.74937962963</v>
+        <v>44076.749379629633</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>45</v>
@@ -2240,7 +2241,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="2">
-        <v>6602.0</v>
+        <v>6602</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>47</v>
@@ -2255,7 +2256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>44076.74961457176</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>51</v>
       </c>
       <c r="D11" s="2">
-        <v>1818672.0</v>
+        <v>1818672</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>52</v>
@@ -2278,9 +2279,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44076.7496674537</v>
+        <v>44076.749667453703</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>53</v>
@@ -2289,7 +2290,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="2">
-        <v>7371.0</v>
+        <v>7371</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>55</v>
@@ -2304,9 +2305,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44076.74981958333</v>
+        <v>44076.749819583332</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>56</v>
@@ -2315,7 +2316,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="2">
-        <v>6330.0</v>
+        <v>6330</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>58</v>
@@ -2330,7 +2331,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>44076.750971180554</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>60</v>
       </c>
       <c r="D14" s="2">
-        <v>9545.0</v>
+        <v>9545</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>61</v>
@@ -2356,9 +2357,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44076.75099180556</v>
+        <v>44076.750991805558</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>63</v>
@@ -2367,7 +2368,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="2">
-        <v>1973.0</v>
+        <v>1973</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>65</v>
@@ -2382,9 +2383,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>44076.75118368056</v>
+        <v>44076.751183680557</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>66</v>
@@ -2393,7 +2394,7 @@
         <v>67</v>
       </c>
       <c r="D16" s="2">
-        <v>6298.0</v>
+        <v>6298</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>68</v>
@@ -2408,9 +2409,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>44076.75165868056</v>
+        <v>44076.751658680558</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>69</v>
@@ -2419,7 +2420,7 @@
         <v>70</v>
       </c>
       <c r="D17" s="2">
-        <v>6092.0</v>
+        <v>6092</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>71</v>
@@ -2434,7 +2435,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>44076.751734641206</v>
       </c>
@@ -2445,7 +2446,7 @@
         <v>46</v>
       </c>
       <c r="D18" s="2">
-        <v>7395.0</v>
+        <v>7395</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>73</v>
@@ -2460,7 +2461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>44076.75174</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>75</v>
       </c>
       <c r="D19" s="2">
-        <v>7304.0</v>
+        <v>7304</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>76</v>
@@ -2486,7 +2487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>44076.751847465275</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>78</v>
       </c>
       <c r="D20" s="2">
-        <v>3305.0</v>
+        <v>3305</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>79</v>
@@ -2512,7 +2513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>44076.751981249996</v>
       </c>
@@ -2523,7 +2524,7 @@
         <v>81</v>
       </c>
       <c r="D21" s="2">
-        <v>3643.0</v>
+        <v>3643</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>82</v>
@@ -2538,7 +2539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>44076.752956435186</v>
       </c>
@@ -2564,9 +2565,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>44076.75298722222</v>
+        <v>44076.752987222222</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>87</v>
@@ -2575,7 +2576,7 @@
         <v>88</v>
       </c>
       <c r="D23" s="2">
-        <v>9127.0</v>
+        <v>9127</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>89</v>
@@ -2590,9 +2591,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>44076.7530666088</v>
+        <v>44076.753066608799</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>91</v>
@@ -2601,7 +2602,7 @@
         <v>92</v>
       </c>
       <c r="D24" s="2">
-        <v>8724.0</v>
+        <v>8724</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>93</v>
@@ -2616,9 +2617,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
-        <v>44076.75314327546</v>
+        <v>44076.753143275462</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>94</v>
@@ -2627,7 +2628,7 @@
         <v>95</v>
       </c>
       <c r="D25" s="2">
-        <v>8382.0</v>
+        <v>8382</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>96</v>
@@ -2642,9 +2643,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>44076.75331659723</v>
+        <v>44076.753316597227</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>97</v>
@@ -2653,7 +2654,7 @@
         <v>98</v>
       </c>
       <c r="D26" s="2">
-        <v>3444.0</v>
+        <v>3444</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>99</v>
@@ -2668,7 +2669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>44076.753444745365</v>
       </c>
@@ -2679,7 +2680,7 @@
         <v>101</v>
       </c>
       <c r="D27" s="2">
-        <v>2915.0</v>
+        <v>2915</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>102</v>
@@ -2694,7 +2695,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>44076.753722442125</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>105</v>
       </c>
       <c r="D28" s="2">
-        <v>7680.0</v>
+        <v>7680</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>106</v>
@@ -2720,7 +2721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>44076.75386217593</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>108</v>
       </c>
       <c r="D29" s="2">
-        <v>5851.0</v>
+        <v>5851</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>109</v>
@@ -2746,9 +2747,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>44076.75392820602</v>
+        <v>44076.753928206017</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>111</v>
@@ -2757,7 +2758,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="2">
-        <v>6821.0</v>
+        <v>6821</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>113</v>
@@ -2772,9 +2773,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>44076.75431952546</v>
+        <v>44076.754319525462</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>114</v>
@@ -2783,7 +2784,7 @@
         <v>115</v>
       </c>
       <c r="D31" s="2">
-        <v>7038.0</v>
+        <v>7038</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>116</v>
@@ -2798,9 +2799,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>44076.75450688657</v>
+        <v>44076.754506886573</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>117</v>
@@ -2809,7 +2810,7 @@
         <v>118</v>
       </c>
       <c r="D32" s="2">
-        <v>1114.0</v>
+        <v>1114</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>119</v>
@@ -2824,9 +2825,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
-        <v>44076.75462903935</v>
+        <v>44076.754629039351</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>120</v>
@@ -2835,7 +2836,7 @@
         <v>121</v>
       </c>
       <c r="D33" s="2">
-        <v>1087.0</v>
+        <v>1087</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>122</v>
@@ -2850,9 +2851,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
-        <v>44076.75468355324</v>
+        <v>44076.754683553241</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>123</v>
@@ -2861,7 +2862,7 @@
         <v>124</v>
       </c>
       <c r="D34" s="2">
-        <v>5010.0</v>
+        <v>5010</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>125</v>
@@ -2876,9 +2877,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
-        <v>44076.75470767361</v>
+        <v>44076.754707673608</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>126</v>
@@ -2887,7 +2888,7 @@
         <v>64</v>
       </c>
       <c r="D35" s="2">
-        <v>3690.0</v>
+        <v>3690</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>127</v>
@@ -2902,9 +2903,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
-        <v>44076.75471324074</v>
+        <v>44076.754713240742</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>128</v>
@@ -2913,7 +2914,7 @@
         <v>129</v>
       </c>
       <c r="D36" s="2">
-        <v>4379.0</v>
+        <v>4379</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>130</v>
@@ -2928,9 +2929,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
-        <v>44076.75577751157</v>
+        <v>44076.755777511571</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>131</v>
@@ -2939,7 +2940,7 @@
         <v>132</v>
       </c>
       <c r="D37" s="2">
-        <v>1761.0</v>
+        <v>1761</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>133</v>
@@ -2954,9 +2955,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
-        <v>44076.75792712963</v>
+        <v>44076.757927129627</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>134</v>
@@ -2965,7 +2966,7 @@
         <v>135</v>
       </c>
       <c r="D38" s="2">
-        <v>8708.0</v>
+        <v>8708</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>136</v>
@@ -2980,9 +2981,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
-        <v>44076.76246215278</v>
+        <v>44076.762462152779</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>137</v>
@@ -2991,7 +2992,7 @@
         <v>138</v>
       </c>
       <c r="D39" s="2">
-        <v>7402.0</v>
+        <v>7402</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>139</v>
@@ -3006,7 +3007,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>44076.766646585646</v>
       </c>
@@ -3017,7 +3018,7 @@
         <v>141</v>
       </c>
       <c r="D40" s="2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>142</v>
@@ -3032,7 +3033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>44076.766863993056</v>
       </c>
@@ -3043,7 +3044,7 @@
         <v>60</v>
       </c>
       <c r="D41" s="2">
-        <v>9545.0</v>
+        <v>9545</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>61</v>
@@ -3058,9 +3059,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
-        <v>44076.7679190625</v>
+        <v>44076.767919062499</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>80</v>
@@ -3069,7 +3070,7 @@
         <v>81</v>
       </c>
       <c r="D42" s="2">
-        <v>3643.0</v>
+        <v>3643</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>82</v>
@@ -3084,7 +3085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>44076.768450902775</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>60</v>
       </c>
       <c r="D43" s="2">
-        <v>9545.0</v>
+        <v>9545</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>61</v>
@@ -3113,9 +3114,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
-        <v>44076.77872325231</v>
+        <v>44076.778723252311</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>63</v>
@@ -3124,7 +3125,7 @@
         <v>64</v>
       </c>
       <c r="D44" s="2">
-        <v>1973.0</v>
+        <v>1973</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>65</v>
@@ -3139,7 +3140,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>44076.778833344906</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>60</v>
       </c>
       <c r="D45" s="2">
-        <v>9545.0</v>
+        <v>9545</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>61</v>
@@ -3168,9 +3169,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
-        <v>44076.78034236111</v>
+        <v>44076.780342361111</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>144</v>
@@ -3194,9 +3195,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
-        <v>44076.78919848379</v>
+        <v>44076.789198483792</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>16</v>
@@ -3205,7 +3206,7 @@
         <v>17</v>
       </c>
       <c r="D47" s="2">
-        <v>4175.0</v>
+        <v>4175</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>18</v>
@@ -3223,9 +3224,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
-        <v>44076.79072314815</v>
+        <v>44076.790723148151</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>147</v>
@@ -3249,7 +3250,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>44076.794545972225</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>51</v>
       </c>
       <c r="D49" s="2">
-        <v>1818672.0</v>
+        <v>1818672</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>52</v>
@@ -3272,9 +3273,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
-        <v>44076.79632601852</v>
+        <v>44076.796326018521</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>151</v>
@@ -3283,7 +3284,7 @@
         <v>108</v>
       </c>
       <c r="D50" s="2">
-        <v>8870.0</v>
+        <v>8870</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>152</v>
@@ -3298,7 +3299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>44076.798428888884</v>
       </c>
@@ -3309,7 +3310,7 @@
         <v>154</v>
       </c>
       <c r="D51" s="2">
-        <v>3697.0</v>
+        <v>3697</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>155</v>
@@ -3324,9 +3325,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
-        <v>44076.80535767361</v>
+        <v>44076.805357673613</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>156</v>
@@ -3335,7 +3336,7 @@
         <v>157</v>
       </c>
       <c r="D52" s="2">
-        <v>6264.0</v>
+        <v>6264</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>158</v>
@@ -3350,9 +3351,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
-        <v>44077.61568321759</v>
+        <v>44077.615683217591</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>153</v>
@@ -3361,7 +3362,7 @@
         <v>154</v>
       </c>
       <c r="D53" s="2">
-        <v>3697.0</v>
+        <v>3697</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>155</v>
@@ -3376,7 +3377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>44080.585858969906</v>
       </c>
@@ -3402,9 +3403,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
-        <v>44083.5003009838</v>
+        <v>44083.500300983796</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>159</v>
@@ -3413,7 +3414,7 @@
         <v>160</v>
       </c>
       <c r="D55" s="2">
-        <v>6264.0</v>
+        <v>6264</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>161</v>
@@ -3428,9 +3429,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
-        <v>44084.47776761574</v>
+        <v>44084.477767615739</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>159</v>
@@ -3439,7 +3440,7 @@
         <v>160</v>
       </c>
       <c r="D56" s="2">
-        <v>6264.0</v>
+        <v>6264</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>161</v>
@@ -3454,9 +3455,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
-        <v>44084.57790621527</v>
+        <v>44084.577906215272</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>163</v>
@@ -3465,7 +3466,7 @@
         <v>164</v>
       </c>
       <c r="D57" s="2">
-        <v>9066.0</v>
+        <v>9066</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>165</v>
@@ -3481,27 +3482,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="15" width="21.57"/>
+    <col min="1" max="15" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3530,9 +3532,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>44103.78968136574</v>
+        <v>44103.789681365743</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -3544,7 +3546,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>5156.0</v>
+        <v>5156</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -3559,9 +3561,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>44103.78982467593</v>
+        <v>44103.789824675929</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>167</v>
@@ -3588,9 +3590,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44103.79001236111</v>
+        <v>44103.790012361111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
@@ -3602,7 +3604,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2">
-        <v>4175.0</v>
+        <v>4175</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -3617,9 +3619,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44103.79023021991</v>
+        <v>44103.790230219907</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>173</v>
@@ -3646,9 +3648,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44104.74566550926</v>
+        <v>44104.745665509261</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -3660,7 +3662,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>4175.0</v>
+        <v>4175</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -3675,9 +3677,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
-        <v>44104.74586607639</v>
+        <v>44104.745866076388</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>114</v>
@@ -3689,7 +3691,7 @@
         <v>116</v>
       </c>
       <c r="E7" s="2">
-        <v>7038.0</v>
+        <v>7038</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>33</v>
@@ -3701,7 +3703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44104.746960833334</v>
       </c>
@@ -3715,7 +3717,7 @@
         <v>127</v>
       </c>
       <c r="E8" s="2">
-        <v>3690.0</v>
+        <v>3690</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>43</v>
@@ -3727,9 +3729,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44104.74779270834</v>
+        <v>44104.747792708338</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>178</v>
@@ -3741,7 +3743,7 @@
         <v>180</v>
       </c>
       <c r="E9" s="2">
-        <v>2665.0</v>
+        <v>2665</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>12</v>
@@ -3753,7 +3755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>44104.748443379634</v>
       </c>
@@ -3767,7 +3769,7 @@
         <v>181</v>
       </c>
       <c r="E10" s="2">
-        <v>5641.0</v>
+        <v>5641</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -3782,7 +3784,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>44104.748588946764</v>
       </c>
@@ -3796,7 +3798,7 @@
         <v>183</v>
       </c>
       <c r="E11" s="2">
-        <v>7680.0</v>
+        <v>7680</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>43</v>
@@ -3808,7 +3810,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>44104.748820925925</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>185</v>
       </c>
       <c r="E12" s="2">
-        <v>9898.0</v>
+        <v>9898</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>12</v>
@@ -3834,9 +3836,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44104.74958042824</v>
+        <v>44104.749580428237</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>186</v>
@@ -3848,7 +3850,7 @@
         <v>187</v>
       </c>
       <c r="E13" s="2">
-        <v>8071.0</v>
+        <v>8071</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>12</v>
@@ -3857,7 +3859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>44104.750114560185</v>
       </c>
@@ -3880,9 +3882,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44104.75060061342</v>
+        <v>44104.750600613421</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>39</v>
@@ -3903,9 +3905,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>44104.75193024306</v>
+        <v>44104.751930243059</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
@@ -3917,7 +3919,7 @@
         <v>190</v>
       </c>
       <c r="E16" s="2">
-        <v>6921.0</v>
+        <v>6921</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>12</v>
@@ -3926,7 +3928,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>44104.752264780094</v>
       </c>
@@ -3940,7 +3942,7 @@
         <v>71</v>
       </c>
       <c r="E17" s="2">
-        <v>6092.0</v>
+        <v>6092</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>12</v>
@@ -3952,9 +3954,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>44104.75254739584</v>
+        <v>44104.752547395838</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>193</v>
@@ -3966,7 +3968,7 @@
         <v>195</v>
       </c>
       <c r="E18" s="2">
-        <v>5819.0</v>
+        <v>5819</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>12</v>
@@ -3978,9 +3980,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>44104.75286305556</v>
+        <v>44104.752863055561</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>196</v>
@@ -3992,7 +3994,7 @@
         <v>198</v>
       </c>
       <c r="E19" s="2">
-        <v>2836.0</v>
+        <v>2836</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>33</v>
@@ -4007,9 +4009,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>44104.75339748843</v>
+        <v>44104.753397488428</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>123</v>
@@ -4021,7 +4023,7 @@
         <v>200</v>
       </c>
       <c r="E20" s="2">
-        <v>5010.0</v>
+        <v>5010</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>48</v>
@@ -4033,9 +4035,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>44104.75420090278</v>
+        <v>44104.754200902782</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>201</v>
@@ -4047,7 +4049,7 @@
         <v>203</v>
       </c>
       <c r="E21" s="2">
-        <v>2200.0</v>
+        <v>2200</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>48</v>
@@ -4059,7 +4061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>44104.754350347226</v>
       </c>
@@ -4073,7 +4075,7 @@
         <v>206</v>
       </c>
       <c r="E22" s="2">
-        <v>8636.0</v>
+        <v>8636</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>12</v>
@@ -4082,9 +4084,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>44104.75575829861</v>
+        <v>44104.755758298612</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>207</v>
@@ -4096,7 +4098,7 @@
         <v>209</v>
       </c>
       <c r="E23" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>33</v>
@@ -4108,9 +4110,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>44104.77384545139</v>
+        <v>44104.773845451389</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>210</v>
@@ -4122,7 +4124,7 @@
         <v>212</v>
       </c>
       <c r="E24" s="2">
-        <v>8138.0</v>
+        <v>8138</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>12</v>
@@ -4131,7 +4133,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>44104.774526064815</v>
       </c>
@@ -4145,7 +4147,7 @@
         <v>213</v>
       </c>
       <c r="E25" s="2">
-        <v>5510.0</v>
+        <v>5510</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>33</v>
@@ -4157,7 +4159,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>44104.77470248843</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>216</v>
       </c>
       <c r="E26" s="2">
-        <v>7686.0</v>
+        <v>7686</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>12</v>
@@ -4183,9 +4185,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
-        <v>44104.80656479167</v>
+        <v>44104.806564791666</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>66</v>
@@ -4197,7 +4199,7 @@
         <v>217</v>
       </c>
       <c r="E27" s="2">
-        <v>6298.0</v>
+        <v>6298</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>12</v>
@@ -4206,9 +4208,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>44104.80713446759</v>
+        <v>44104.807134467592</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>153</v>
@@ -4220,7 +4222,7 @@
         <v>155</v>
       </c>
       <c r="E28" s="2">
-        <v>9637.0</v>
+        <v>9637</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>12</v>
@@ -4232,9 +4234,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
-        <v>44104.84373424768</v>
+        <v>44104.843734247683</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>207</v>
@@ -4246,7 +4248,7 @@
         <v>209</v>
       </c>
       <c r="E29" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>33</v>
@@ -4258,9 +4260,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>44105.73901319444</v>
+        <v>44105.739013194441</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>191</v>
@@ -4272,7 +4274,7 @@
         <v>71</v>
       </c>
       <c r="E30" s="2">
-        <v>6092.0</v>
+        <v>6092</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>12</v>
@@ -4284,9 +4286,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>44105.89238546297</v>
+        <v>44105.892385462968</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>207</v>
@@ -4298,7 +4300,7 @@
         <v>209</v>
       </c>
       <c r="E31" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>33</v>
@@ -4310,7 +4312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>44175.39098488426</v>
       </c>
@@ -4324,7 +4326,7 @@
         <v>209</v>
       </c>
       <c r="E32" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>33</v>
@@ -4336,7 +4338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>44202.54766650463</v>
       </c>
@@ -4350,7 +4352,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="2">
-        <v>4175.0</v>
+        <v>4175</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>19</v>
@@ -4366,27 +4368,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="15" width="21.57"/>
+    <col min="1" max="15" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4415,9 +4418,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>44126.73654837963</v>
+        <v>44126.736548379631</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -4429,7 +4432,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>5256.0</v>
+        <v>5256</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -4444,9 +4447,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>44126.75339825232</v>
+        <v>44126.753398252316</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>210</v>
@@ -4458,7 +4461,7 @@
         <v>219</v>
       </c>
       <c r="E3" s="2">
-        <v>8138.0</v>
+        <v>8138</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -4470,9 +4473,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44126.75360707176</v>
+        <v>44126.753607071762</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>220</v>
@@ -4484,7 +4487,7 @@
         <v>221</v>
       </c>
       <c r="E4" s="2">
-        <v>7882.0</v>
+        <v>7882</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>43</v>
@@ -4496,9 +4499,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44126.75364060185</v>
+        <v>44126.753640601848</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>222</v>
@@ -4510,7 +4513,7 @@
         <v>224</v>
       </c>
       <c r="E5" s="2">
-        <v>5933.0</v>
+        <v>5933</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -4525,9 +4528,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44126.75383502315</v>
+        <v>44126.753835023148</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>196</v>
@@ -4539,7 +4542,7 @@
         <v>226</v>
       </c>
       <c r="E6" s="2">
-        <v>2836.0</v>
+        <v>2836</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>33</v>
@@ -4554,7 +4557,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>44126.753939131944</v>
       </c>
@@ -4568,7 +4571,7 @@
         <v>102</v>
       </c>
       <c r="E7" s="2">
-        <v>2915.0</v>
+        <v>2915</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>33</v>
@@ -4580,7 +4583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44126.754057928236</v>
       </c>
@@ -4594,7 +4597,7 @@
         <v>230</v>
       </c>
       <c r="E8" s="2">
-        <v>8732.0</v>
+        <v>8732</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>12</v>
@@ -4606,9 +4609,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44126.75412400463</v>
+        <v>44126.754124004627</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>231</v>
@@ -4620,7 +4623,7 @@
         <v>233</v>
       </c>
       <c r="E9" s="2">
-        <v>2059.0</v>
+        <v>2059</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>43</v>
@@ -4632,7 +4635,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>44126.754448900465</v>
       </c>
@@ -4646,7 +4649,7 @@
         <v>236</v>
       </c>
       <c r="E10" s="2">
-        <v>8967.0</v>
+        <v>8967</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>110</v>
@@ -4658,9 +4661,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>44126.75457074074</v>
+        <v>44126.754570740741</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>39</v>
@@ -4684,9 +4687,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44126.75463648148</v>
+        <v>44126.754636481477</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -4707,9 +4710,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44126.75481168981</v>
+        <v>44126.754811689811</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>104</v>
@@ -4721,7 +4724,7 @@
         <v>238</v>
       </c>
       <c r="E13" s="2">
-        <v>7680.0</v>
+        <v>7680</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>43</v>
@@ -4733,9 +4736,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>44126.75666371528</v>
+        <v>44126.756663715278</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>239</v>
@@ -4747,7 +4750,7 @@
         <v>241</v>
       </c>
       <c r="E14" s="2">
-        <v>8007.0</v>
+        <v>8007</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>12</v>
@@ -4759,9 +4762,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44126.75782814815</v>
+        <v>44126.757828148147</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>242</v>
@@ -4785,9 +4788,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>44126.75820859954</v>
+        <v>44126.758208599538</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>207</v>
@@ -4799,7 +4802,7 @@
         <v>246</v>
       </c>
       <c r="E16" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>33</v>
@@ -4811,9 +4814,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>44126.75918304398</v>
+        <v>44126.759183043978</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
@@ -4825,7 +4828,7 @@
         <v>181</v>
       </c>
       <c r="E17" s="2">
-        <v>5641.0</v>
+        <v>5641</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>12</v>
@@ -4837,9 +4840,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>44126.75919318287</v>
+        <v>44126.759193182872</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>126</v>
@@ -4851,7 +4854,7 @@
         <v>127</v>
       </c>
       <c r="E18" s="2">
-        <v>3690.0</v>
+        <v>3690</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>43</v>
@@ -4860,7 +4863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>44126.759702916665</v>
       </c>
@@ -4874,7 +4877,7 @@
         <v>247</v>
       </c>
       <c r="E19" s="2">
-        <v>9637.0</v>
+        <v>9637</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>12</v>
@@ -4886,7 +4889,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>44127.163216030094</v>
       </c>
@@ -4900,7 +4903,7 @@
         <v>246</v>
       </c>
       <c r="E20" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>33</v>
@@ -4912,9 +4915,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>44129.03444866899</v>
+        <v>44129.034448668986</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>231</v>
@@ -4926,7 +4929,7 @@
         <v>233</v>
       </c>
       <c r="E21" s="2">
-        <v>2059.0</v>
+        <v>2059</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>43</v>
@@ -4938,9 +4941,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>44129.84749684027</v>
+        <v>44129.847496840273</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>100</v>
@@ -4952,7 +4955,7 @@
         <v>102</v>
       </c>
       <c r="E22" s="2">
-        <v>2915.0</v>
+        <v>2915</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>33</v>
@@ -4966,29 +4969,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D19"/>
+    <hyperlink ref="D19" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="15" width="21.57"/>
+    <col min="1" max="15" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5017,7 +5021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>44154.605010555555</v>
       </c>
@@ -5031,7 +5035,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>5156.0</v>
+        <v>5156</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -5046,9 +5050,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>44154.74690570602</v>
+        <v>44154.746905706023</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>196</v>
@@ -5060,7 +5064,7 @@
         <v>226</v>
       </c>
       <c r="E3" s="2">
-        <v>2836.0</v>
+        <v>2836</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>33</v>
@@ -5072,7 +5076,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>44154.747910844904</v>
       </c>
@@ -5086,7 +5090,7 @@
         <v>250</v>
       </c>
       <c r="E4" s="2">
-        <v>8732.0</v>
+        <v>8732</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>12</v>
@@ -5098,9 +5102,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44154.74799108796</v>
+        <v>44154.747991087963</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -5112,7 +5116,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="2">
-        <v>5641.0</v>
+        <v>5641</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -5127,9 +5131,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44154.74806416666</v>
+        <v>44154.748064166663</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>252</v>
@@ -5141,7 +5145,7 @@
         <v>253</v>
       </c>
       <c r="E6" s="2">
-        <v>9898.0</v>
+        <v>9898</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>
@@ -5153,7 +5157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>44154.748188171296</v>
       </c>
@@ -5167,7 +5171,7 @@
         <v>254</v>
       </c>
       <c r="E7" s="2">
-        <v>7680.0</v>
+        <v>7680</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>43</v>
@@ -5179,7 +5183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44154.748195196764</v>
       </c>
@@ -5193,7 +5197,7 @@
         <v>209</v>
       </c>
       <c r="E8" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>33</v>
@@ -5205,9 +5209,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44154.74830075231</v>
+        <v>44154.748300752311</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>83</v>
@@ -5231,7 +5235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>44154.749560543976</v>
       </c>
@@ -5245,7 +5249,7 @@
         <v>116</v>
       </c>
       <c r="E10" s="2">
-        <v>7038.0</v>
+        <v>7038</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>33</v>
@@ -5260,9 +5264,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>44154.74986023148</v>
+        <v>44154.749860231481</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>36</v>
@@ -5286,9 +5290,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44154.75008174768</v>
+        <v>44154.750081747683</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>222</v>
@@ -5300,7 +5304,7 @@
         <v>224</v>
       </c>
       <c r="E12" s="2">
-        <v>5933.0</v>
+        <v>5933</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>12</v>
@@ -5312,9 +5316,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44154.75112943287</v>
+        <v>44154.751129432872</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>259</v>
@@ -5326,7 +5330,7 @@
         <v>260</v>
       </c>
       <c r="E13" s="2">
-        <v>6941.0</v>
+        <v>6941</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>12</v>
@@ -5341,9 +5345,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>44154.75228892361</v>
+        <v>44154.752288923613</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>151</v>
@@ -5355,7 +5359,7 @@
         <v>262</v>
       </c>
       <c r="E14" s="2">
-        <v>8870.0</v>
+        <v>8870</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>33</v>
@@ -5367,9 +5371,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44154.75295034722</v>
+        <v>44154.752950347218</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>39</v>
@@ -5393,7 +5397,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>44154.753233599535</v>
       </c>
@@ -5407,7 +5411,7 @@
         <v>263</v>
       </c>
       <c r="E16" s="2">
-        <v>6092.0</v>
+        <v>6092</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>12</v>
@@ -5419,7 +5423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>44154.753811041664</v>
       </c>
@@ -5433,7 +5437,7 @@
         <v>68</v>
       </c>
       <c r="E17" s="2">
-        <v>6298.0</v>
+        <v>6298</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>12</v>
@@ -5442,7 +5446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>44154.754273252314</v>
       </c>
@@ -5456,7 +5460,7 @@
         <v>266</v>
       </c>
       <c r="E18" s="2">
-        <v>8618.0</v>
+        <v>8618</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>12</v>
@@ -5468,7 +5472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>44154.755732314814</v>
       </c>
@@ -5482,7 +5486,7 @@
         <v>269</v>
       </c>
       <c r="E19" s="2">
-        <v>1052.0</v>
+        <v>1052</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>43</v>
@@ -5497,9 +5501,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>44154.76010886574</v>
+        <v>44154.760108865739</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>271</v>
@@ -5511,7 +5515,7 @@
         <v>273</v>
       </c>
       <c r="E20" s="2">
-        <v>7955.0</v>
+        <v>7955</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>19</v>
@@ -5523,9 +5527,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>44154.76997890046</v>
+        <v>44154.769978900462</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>210</v>
@@ -5537,7 +5541,7 @@
         <v>219</v>
       </c>
       <c r="E21" s="2">
-        <v>8138.0</v>
+        <v>8138</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>12</v>
@@ -5549,9 +5553,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>44154.79563087963</v>
+        <v>44154.795630879627</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>275</v>
@@ -5563,7 +5567,7 @@
         <v>277</v>
       </c>
       <c r="E22" s="2">
-        <v>8522.0</v>
+        <v>8522</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>43</v>
@@ -5575,7 +5579,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>44154.960660462966</v>
       </c>
@@ -5589,7 +5593,7 @@
         <v>224</v>
       </c>
       <c r="E23" s="2">
-        <v>5933.0</v>
+        <v>5933</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>12</v>
@@ -5601,9 +5605,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>44156.92734789352</v>
+        <v>44156.927347893521</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>207</v>
@@ -5615,7 +5619,7 @@
         <v>209</v>
       </c>
       <c r="E24" s="2">
-        <v>8876.0</v>
+        <v>8876</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>33</v>
@@ -5627,9 +5631,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
-        <v>44159.30287745371</v>
+        <v>44159.302877453709</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>271</v>
@@ -5641,7 +5645,7 @@
         <v>273</v>
       </c>
       <c r="E25" s="2">
-        <v>7955.0</v>
+        <v>7955</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>19</v>
@@ -5653,7 +5657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>44185.340399733795</v>
       </c>
@@ -5667,7 +5671,7 @@
         <v>277</v>
       </c>
       <c r="E26" s="2">
-        <v>8522.0</v>
+        <v>8522</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>43</v>
@@ -5680,29 +5684,30 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="21.57"/>
-    <col customWidth="1" min="5" max="5" width="396.14"/>
-    <col customWidth="1" min="6" max="12" width="21.57"/>
+    <col min="1" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="396.1640625" customWidth="1"/>
+    <col min="6" max="12" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5722,7 +5727,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>44130.588415439815</v>
       </c>
@@ -5742,9 +5747,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>44130.60961079861</v>
+        <v>44130.609610798609</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>285</v>
@@ -5762,9 +5767,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44130.61053961806</v>
+        <v>44130.610539618057</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>288</v>
@@ -5782,9 +5787,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44130.76505096065</v>
+        <v>44130.765050960646</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>292</v>
@@ -5802,9 +5807,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44130.83097510417</v>
+        <v>44130.830975104167</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>295</v>
@@ -5822,7 +5827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>44131.507554571755</v>
       </c>
@@ -5842,9 +5847,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
-        <v>44131.54355320602</v>
+        <v>44131.543553206022</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>301</v>
@@ -5862,9 +5867,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44131.67295609954</v>
+        <v>44131.672956099537</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>304</v>
@@ -5882,7 +5887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>44131.737349560186</v>
       </c>
@@ -5902,7 +5907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>44131.798752118055</v>
       </c>
@@ -5922,9 +5927,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44131.83327717593</v>
+        <v>44131.833277175931</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>313</v>
@@ -5942,7 +5947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>44132.716859513894</v>
       </c>
@@ -5962,9 +5967,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>44132.8142590162</v>
+        <v>44132.814259016202</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>304</v>
@@ -5982,9 +5987,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44133.54634777778</v>
+        <v>44133.546347777781</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>318</v>
@@ -6002,9 +6007,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>44137.50565769676</v>
+        <v>44137.505657696762</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>321</v>
@@ -6022,9 +6027,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>44127.62570225695</v>
+        <v>44127.625702256948</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>64</v>
@@ -6042,9 +6047,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>44127.6328178588</v>
+        <v>44127.632817858801</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>229</v>
@@ -6062,9 +6067,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>44127.68999616898</v>
+        <v>44127.689996168978</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>194</v>
@@ -6082,9 +6087,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>44127.73794755787</v>
+        <v>44127.737947557871</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>326</v>
@@ -6102,9 +6107,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>44128.32577488426</v>
+        <v>44128.325774884259</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>329</v>
@@ -6122,9 +6127,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>44128.52733810185</v>
+        <v>44128.527338101849</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>281</v>
@@ -6142,9 +6147,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>44129.85848634259</v>
+        <v>44129.858486342593</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>332</v>
@@ -6162,9 +6167,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>44130.58858675926</v>
+        <v>44130.588586759259</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>179</v>
@@ -6182,9 +6187,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
-        <v>44130.60403266204</v>
+        <v>44130.604032662042</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>337</v>
@@ -6202,9 +6207,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>44130.61354320602</v>
+        <v>44130.613543206018</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>340</v>
@@ -6222,9 +6227,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
-        <v>44130.63737</v>
+        <v>44130.637369999997</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>342</v>
@@ -6242,9 +6247,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>44130.82507545139</v>
+        <v>44130.825075451387</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>345</v>
@@ -6262,7 +6267,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>44131.91715814815</v>
       </c>
@@ -6282,9 +6287,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>44133.28097103009</v>
+        <v>44133.280971030093</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>348</v>
@@ -6302,9 +6307,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>44133.95513015046</v>
+        <v>44133.955130150462</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>347</v>
@@ -6322,9 +6327,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>44137.38210149306</v>
+        <v>44137.382101493058</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>92</v>
@@ -6342,7 +6347,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>44137.437596504635</v>
       </c>
@@ -6362,9 +6367,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
-        <v>44137.68076556713</v>
+        <v>44137.680765567129</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>351</v>
@@ -6382,7 +6387,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>44137.71536829861</v>
       </c>
@@ -6402,7 +6407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>44136.583308229165</v>
       </c>
@@ -6419,9 +6424,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
-        <v>44139.19282689814</v>
+        <v>44139.192826898143</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>355</v>
@@ -6437,27 +6442,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="10" width="21.57"/>
+    <col min="1" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6471,49 +6477,49 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>44130.7484452662</v>
+        <v>44130.748445266203</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>361</v>
       </c>
       <c r="C2" s="2">
-        <v>1052.0</v>
+        <v>1052</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>44130.75111075232</v>
+        <v>44130.751110752317</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>362</v>
       </c>
       <c r="C3" s="2">
-        <v>9898.0</v>
+        <v>9898</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44130.7567228125</v>
+        <v>44130.756722812497</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>363</v>
       </c>
       <c r="C4" s="2">
-        <v>9504.0</v>
+        <v>9504</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>44130.757522858796</v>
       </c>
@@ -6521,39 +6527,40 @@
         <v>365</v>
       </c>
       <c r="C5" s="2">
-        <v>2665.0</v>
+        <v>2665</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>283</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="21.57"/>
-    <col customWidth="1" min="4" max="4" width="31.71"/>
-    <col customWidth="1" hidden="1" min="5" max="5" width="29.0"/>
-    <col customWidth="1" min="6" max="6" width="92.29"/>
-    <col customWidth="1" min="7" max="7" width="38.86"/>
-    <col customWidth="1" min="8" max="13" width="21.57"/>
+    <col min="1" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="92.33203125" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" customWidth="1"/>
+    <col min="8" max="13" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6576,9 +6583,9 @@
         <v>369</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>44060.74746438657</v>
+        <v>44060.747464386572</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>370</v>
@@ -6599,7 +6606,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>44074.483493796295</v>
       </c>
@@ -6622,9 +6629,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44074.58690070602</v>
+        <v>44074.586900706017</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>378</v>
@@ -6645,9 +6652,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44074.61269547454</v>
+        <v>44074.612695474541</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>382</v>
@@ -6668,7 +6675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>44060.653495763894</v>
       </c>
@@ -6691,9 +6698,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
-        <v>44073.89569228009</v>
+        <v>44073.895692280093</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>390</v>
@@ -6714,7 +6721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44061.134752881946</v>
       </c>
@@ -6737,9 +6744,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44063.3931815625</v>
+        <v>44063.393181562496</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>141</v>
@@ -6760,7 +6767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>44075.49323216435</v>
       </c>
@@ -6783,9 +6790,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>44060.71242996528</v>
+        <v>44060.712429965279</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>95</v>
@@ -6806,9 +6813,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44061.37123554398</v>
+        <v>44061.371235543978</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>406</v>
@@ -6829,40 +6836,41 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="13" width="21.57"/>
+    <col min="1" max="13" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6894,7 +6902,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>44069.432835740736</v>
       </c>
@@ -6914,20 +6922,20 @@
         <v>420</v>
       </c>
       <c r="H2" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I2" s="6">
-        <v>0.5208333333333334</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="J2" s="7">
-        <f t="shared" ref="J2:J41" si="1">I2+H2/(24*60)</f>
-        <v>0.5416666667</v>
+        <f t="shared" ref="J2:J41" si="0">I2+H2/(24*60)</f>
+        <v>0.54166666666666674</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>44069.433114722226</v>
       </c>
@@ -6947,22 +6955,22 @@
         <v>420</v>
       </c>
       <c r="H3" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I3" s="6">
-        <v>0.5208333333333334</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5416666667</v>
+        <f t="shared" si="0"/>
+        <v>0.54166666666666674</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44069.43326925926</v>
+        <v>44069.433269259258</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>425</v>
@@ -6980,22 +6988,22 @@
         <v>429</v>
       </c>
       <c r="H4" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I4" s="6">
-        <v>0.5208333333333334</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="J4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.53125</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44069.43385377315</v>
+        <v>44069.433853773153</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>430</v>
@@ -7016,22 +7024,22 @@
         <v>261</v>
       </c>
       <c r="H5" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I5" s="6">
-        <v>0.5208333333333334</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5416666667</v>
+        <f t="shared" si="0"/>
+        <v>0.54166666666666674</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44069.43480015046</v>
+        <v>44069.434800150462</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>434</v>
@@ -7049,22 +7057,22 @@
         <v>420</v>
       </c>
       <c r="H6" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I6" s="6">
-        <v>0.5208333333333334</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="J6" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5416666667</v>
+        <f t="shared" si="0"/>
+        <v>0.54166666666666674</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
-        <v>44069.43761974537</v>
+        <v>44069.437619745368</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>437</v>
@@ -7082,20 +7090,20 @@
         <v>420</v>
       </c>
       <c r="H7" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I7" s="6">
-        <v>0.5208333333333334</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="J7" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5416666667</v>
+        <f t="shared" si="0"/>
+        <v>0.54166666666666674</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>44069.437804236106</v>
       </c>
@@ -7115,23 +7123,23 @@
         <v>429</v>
       </c>
       <c r="H8" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I8" s="8" t="str">
-        <f t="shared" ref="I8:I24" si="2">text(J2,"H:MM AM/PM")</f>
+        <f t="shared" ref="I8:I24" si="1">TEXT(J2,"H:MM AM/PM")</f>
         <v>1:00 PM</v>
       </c>
       <c r="J8" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5520833333</v>
+        <f t="shared" si="0"/>
+        <v>0.55208333333333326</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44069.44204837963</v>
+        <v>44069.442048379628</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>444</v>
@@ -7149,23 +7157,23 @@
         <v>429</v>
       </c>
       <c r="H9" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I9" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:00 PM</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5520833333</v>
+        <f t="shared" si="0"/>
+        <v>0.55208333333333326</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>44069.45033584491</v>
+        <v>44069.450335844907</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>446</v>
@@ -7183,21 +7191,21 @@
         <v>420</v>
       </c>
       <c r="H10" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I10" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12:45 PM</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5520833333</v>
+        <f t="shared" si="0"/>
+        <v>0.55208333333333337</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>44069.45336373843</v>
       </c>
@@ -7217,23 +7225,23 @@
         <v>420</v>
       </c>
       <c r="H11" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I11" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:00 PM</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5625</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44069.45339609953</v>
+        <v>44069.453396099532</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>453</v>
@@ -7251,23 +7259,23 @@
         <v>420</v>
       </c>
       <c r="H12" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I12" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:00 PM</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5625</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44069.45352924769</v>
+        <v>44069.453529247687</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>456</v>
@@ -7288,23 +7296,23 @@
         <v>459</v>
       </c>
       <c r="H13" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I13" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:00 PM</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5625</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>44069.46202359954</v>
+        <v>44069.462023599539</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>460</v>
@@ -7322,23 +7330,23 @@
         <v>464</v>
       </c>
       <c r="H14" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="I14" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:15 PM</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5659722222</v>
+        <f t="shared" si="0"/>
+        <v>0.56597222222222221</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44069.47071613426</v>
+        <v>44069.470716134259</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>465</v>
@@ -7356,21 +7364,21 @@
         <v>420</v>
       </c>
       <c r="H15" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I15" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:15 PM</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5729166667</v>
+        <f t="shared" si="0"/>
+        <v>0.57291666666666674</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>44069.487366354166</v>
       </c>
@@ -7390,21 +7398,21 @@
         <v>420</v>
       </c>
       <c r="H16" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I16" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:15 PM</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5729166667</v>
+        <f t="shared" si="0"/>
+        <v>0.57291666666666674</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>44069.49346618056</v>
       </c>
@@ -7424,21 +7432,21 @@
         <v>420</v>
       </c>
       <c r="H17" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I17" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:30 PM</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5833333333</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>44069.500050752315</v>
       </c>
@@ -7458,21 +7466,21 @@
         <v>420</v>
       </c>
       <c r="H18" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I18" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:30 PM</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5833333333</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>44069.504346041664</v>
       </c>
@@ -7492,27 +7500,27 @@
         <v>420</v>
       </c>
       <c r="H19" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I19" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1:30 PM</v>
       </c>
       <c r="J19" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5833333333</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
       </c>
       <c r="K19" s="10" t="str">
-        <f t="shared" ref="K19:K24" si="3">text(J19,"H:MM AM/PM")</f>
+        <f t="shared" ref="K19:K24" si="2">TEXT(J19,"H:MM AM/PM")</f>
         <v>2:00 PM</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>44069.5256841088</v>
+        <v>44069.525684108798</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>195</v>
@@ -7530,25 +7538,25 @@
         <v>420</v>
       </c>
       <c r="H20" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I20" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1:35 PM</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="0"/>
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="K20" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>1:35 PM</v>
-      </c>
-      <c r="J20" s="7">
-        <f t="shared" si="1"/>
-        <v>0.5868055556</v>
-      </c>
-      <c r="K20" s="10" t="str">
-        <f t="shared" si="3"/>
         <v>2:05 PM</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>44069.53025924768</v>
       </c>
@@ -7568,27 +7576,27 @@
         <v>420</v>
       </c>
       <c r="H21" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I21" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1:45 PM</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="K21" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>1:45 PM</v>
-      </c>
-      <c r="J21" s="7">
-        <f t="shared" si="1"/>
-        <v>0.59375</v>
-      </c>
-      <c r="K21" s="10" t="str">
-        <f t="shared" si="3"/>
         <v>2:15 PM</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>44069.5464034375</v>
+        <v>44069.546403437504</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>480</v>
@@ -7606,25 +7614,25 @@
         <v>420</v>
       </c>
       <c r="H22" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I22" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1:45 PM</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="K22" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>1:45 PM</v>
-      </c>
-      <c r="J22" s="7">
-        <f t="shared" si="1"/>
-        <v>0.59375</v>
-      </c>
-      <c r="K22" s="10" t="str">
-        <f t="shared" si="3"/>
         <v>2:15 PM</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>44069.570567083334</v>
       </c>
@@ -7647,25 +7655,25 @@
         <v>488</v>
       </c>
       <c r="H23" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I23" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>2:00 PM</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="K23" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>2:00 PM</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="1"/>
-        <v>0.59375</v>
-      </c>
-      <c r="K23" s="10" t="str">
-        <f t="shared" si="3"/>
         <v>2:15 PM</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>44069.610642291664</v>
       </c>
@@ -7685,25 +7693,25 @@
         <v>429</v>
       </c>
       <c r="H24" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I24" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>2:00 PM</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="K24" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>2:00 PM</v>
-      </c>
-      <c r="J24" s="7">
-        <f t="shared" si="1"/>
-        <v>0.59375</v>
-      </c>
-      <c r="K24" s="10" t="str">
-        <f t="shared" si="3"/>
         <v>2:15 PM</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>44069.612336782404</v>
       </c>
@@ -7726,20 +7734,20 @@
         <v>495</v>
       </c>
       <c r="H25" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I25" s="6">
-        <v>0.09722222222222222</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1180555556</v>
+        <f t="shared" si="0"/>
+        <v>0.11805555555555555</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>44069.66495622685</v>
       </c>
@@ -7759,20 +7767,20 @@
         <v>420</v>
       </c>
       <c r="H26" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I26" s="6">
-        <v>0.09722222222222222</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="J26" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1180555556</v>
+        <f t="shared" si="0"/>
+        <v>0.11805555555555555</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>44069.669467326385</v>
       </c>
@@ -7792,20 +7800,20 @@
         <v>420</v>
       </c>
       <c r="H27" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I27" s="6">
-        <v>0.09722222222222222</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="J27" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1180555556</v>
+        <f t="shared" si="0"/>
+        <v>0.11805555555555555</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>44069.66964511574</v>
       </c>
@@ -7825,22 +7833,22 @@
         <v>420</v>
       </c>
       <c r="H28" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I28" s="6">
-        <v>0.09722222222222222</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="J28" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1180555556</v>
+        <f t="shared" si="0"/>
+        <v>0.11805555555555555</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
-        <v>44069.72530967592</v>
+        <v>44069.725309675923</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>507</v>
@@ -7858,22 +7866,22 @@
         <v>420</v>
       </c>
       <c r="H29" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I29" s="6">
-        <v>0.09722222222222222</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="J29" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1180555556</v>
+        <f t="shared" si="0"/>
+        <v>0.11805555555555555</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>44069.76689009259</v>
+        <v>44069.766890092593</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>510</v>
@@ -7891,23 +7899,23 @@
         <v>420</v>
       </c>
       <c r="H30" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I30" s="8" t="str">
-        <f t="shared" ref="I30:I39" si="4">text(J25,"H:MM AM/PM")</f>
+        <f t="shared" ref="I30:I39" si="3">TEXT(J25,"H:MM AM/PM")</f>
         <v>2:50 AM</v>
       </c>
       <c r="J30" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1388888889</v>
+        <f t="shared" si="0"/>
+        <v>0.1388888888888889</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>44070.03806384259</v>
+        <v>44070.038063842592</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>514</v>
@@ -7925,23 +7933,23 @@
         <v>429</v>
       </c>
       <c r="H31" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I31" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2:50 AM</v>
       </c>
       <c r="J31" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1284722222</v>
+        <f t="shared" si="0"/>
+        <v>0.12847222222222224</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>44070.58861226852</v>
+        <v>44070.588612268519</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>52</v>
@@ -7959,23 +7967,23 @@
         <v>420</v>
       </c>
       <c r="H32" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I32" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2:50 AM</v>
       </c>
       <c r="J32" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1388888889</v>
+        <f t="shared" si="0"/>
+        <v>0.1388888888888889</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
-        <v>44070.61788371528</v>
+        <v>44070.617883715277</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>516</v>
@@ -7993,21 +8001,21 @@
         <v>420</v>
       </c>
       <c r="H33" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I33" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2:50 AM</v>
       </c>
       <c r="J33" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1388888889</v>
+        <f t="shared" si="0"/>
+        <v>0.1388888888888889</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>44070.66427818287</v>
       </c>
@@ -8027,23 +8035,23 @@
         <v>420</v>
       </c>
       <c r="H34" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I34" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2:50 AM</v>
       </c>
       <c r="J34" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1388888889</v>
+        <f t="shared" si="0"/>
+        <v>0.1388888888888889</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
-        <v>44071.59941260416</v>
+        <v>44071.599412604162</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>520</v>
@@ -8061,25 +8069,25 @@
         <v>420</v>
       </c>
       <c r="H35" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I35" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3:20 AM</v>
       </c>
       <c r="J35" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1597222222</v>
+        <f t="shared" si="0"/>
+        <v>0.15972222222222224</v>
       </c>
       <c r="K35" s="10" t="str">
-        <f>text(J35,"H:MM AM/PM")</f>
+        <f>TEXT(J35,"H:MM AM/PM")</f>
         <v>3:50 AM</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>44071.605235069444</v>
       </c>
@@ -8099,23 +8107,23 @@
         <v>420</v>
       </c>
       <c r="H36" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I36" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3:05 AM</v>
       </c>
       <c r="J36" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1493055556</v>
+        <f t="shared" si="0"/>
+        <v>0.14930555555555558</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
-        <v>44071.61196550926</v>
+        <v>44071.611965509263</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>525</v>
@@ -8133,27 +8141,27 @@
         <v>420</v>
       </c>
       <c r="H37" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I37" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3:20 AM</v>
       </c>
       <c r="J37" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1597222222</v>
+        <f t="shared" si="0"/>
+        <v>0.15972222222222224</v>
       </c>
       <c r="K37" s="10" t="str">
-        <f t="shared" ref="K37:K38" si="5">text(J37,"H:MM AM/PM")</f>
+        <f t="shared" ref="K37:K38" si="4">TEXT(J37,"H:MM AM/PM")</f>
         <v>3:50 AM</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
-        <v>44072.0517475</v>
+        <v>44072.051747500002</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>528</v>
@@ -8171,25 +8179,25 @@
         <v>420</v>
       </c>
       <c r="H38" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I38" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>3:20 AM</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" si="0"/>
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="K38" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>3:20 AM</v>
-      </c>
-      <c r="J38" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1597222222</v>
-      </c>
-      <c r="K38" s="10" t="str">
-        <f t="shared" si="5"/>
         <v>3:50 AM</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>44072.587256388884</v>
       </c>
@@ -8209,23 +8217,23 @@
         <v>429</v>
       </c>
       <c r="H39" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="I39" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3:20 AM</v>
       </c>
       <c r="J39" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1493055556</v>
+        <f t="shared" si="0"/>
+        <v>0.14930555555555555</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
-        <v>44072.77280494213</v>
+        <v>44072.772804942128</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>533</v>
@@ -8243,27 +8251,27 @@
         <v>464</v>
       </c>
       <c r="H40" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="I40" s="11" t="str">
-        <f>text(J36,"H:MM AM/PM")</f>
+        <f>TEXT(J36,"H:MM AM/PM")</f>
         <v>3:35 AM</v>
       </c>
       <c r="J40" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1631944444</v>
+        <f t="shared" si="0"/>
+        <v>0.16319444444444445</v>
       </c>
       <c r="K40" s="10" t="str">
-        <f t="shared" ref="K40:K41" si="6">text(J40,"H:MM AM/PM")</f>
+        <f t="shared" ref="K40:K41" si="5">TEXT(J40,"H:MM AM/PM")</f>
         <v>3:55 AM</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
-        <v>44072.98965480324</v>
+        <v>44072.989654803241</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>536</v>
@@ -8281,38 +8289,38 @@
         <v>420</v>
       </c>
       <c r="H41" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="I41" s="11" t="str">
-        <f>text(J39,"H:MM AM/PM")</f>
+        <f>TEXT(J39,"H:MM AM/PM")</f>
         <v>3:35 AM</v>
       </c>
       <c r="J41" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1701388889</v>
+        <f t="shared" si="0"/>
+        <v>0.1701388888888889</v>
       </c>
       <c r="K41" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4:05 AM</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="H42" s="1">
-        <f>sum(H1:H41)/60</f>
-        <v>17.91666667</v>
-      </c>
-    </row>
-    <row r="43">
+        <f>SUM(H1:H41)/60</f>
+        <v>17.916666666666668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H43" s="1">
         <f>H42-1.75*9</f>
-        <v>2.166666667</v>
+        <v>2.1666666666666679</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>